<commit_message>
Actualizacion de Cronograma, Informe y Hoja de desempeño
</commit_message>
<xml_diff>
--- a/P3GA1/DocumentosProyecto/Hoja de Desempeño.xlsx
+++ b/P3GA1/DocumentosProyecto/Hoja de Desempeño.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SEBAS\Desktop\P\P3GA1\DocumentosProyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95853613-B92D-403E-9D1F-63311CC723F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{237E3E0D-3D2D-49E0-AF60-BCE99F3F8333}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -796,7 +796,7 @@
                 <c:formatCode>0_);[Red]\(0\)</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>9.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>10</c:v>
@@ -814,7 +814,7 @@
                 <c:formatCode>0_);[Red]\(0\)</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>9.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -889,7 +889,7 @@
                 <c:formatCode>0_);[Red]\(0\)</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>9.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>10</c:v>
@@ -982,7 +982,7 @@
                 <c:formatCode>0_);[Red]\(0\)</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>9.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>10</c:v>
@@ -1103,7 +1103,7 @@
                       <c:formatCode>0_);[Red]\(0\)</c:formatCode>
                       <c:ptCount val="3"/>
                       <c:pt idx="0">
-                        <c:v>10</c:v>
+                        <c:v>9.6</c:v>
                       </c:pt>
                       <c:pt idx="1">
                         <c:v>10</c:v>
@@ -1300,7 +1300,7 @@
                 <c:formatCode>0_);[Red]\(0\)</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>10</c:v>
@@ -1736,7 +1736,7 @@
                 <c:formatCode>0_);[Red]\(0\)</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>10</c:v>
@@ -1888,7 +1888,7 @@
                 <c:formatCode>0_);[Red]\(0\)</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>10</c:v>
@@ -2013,7 +2013,7 @@
                 <c:formatCode>0_);[Red]\(0\)</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>9.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>10</c:v>
@@ -2660,7 +2660,7 @@
   <dimension ref="A1:AF7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AI7" sqref="AI7"/>
+      <selection activeCell="W5" sqref="W5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2851,17 +2851,21 @@
       <c r="B4" s="7">
         <v>10</v>
       </c>
-      <c r="C4" s="30"/>
+      <c r="C4" s="30">
+        <v>8</v>
+      </c>
       <c r="D4" s="30"/>
       <c r="E4" s="30"/>
       <c r="F4" s="14">
         <f>AVERAGE(B4:E4)</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G4" s="8">
         <v>10</v>
       </c>
-      <c r="H4" s="8"/>
+      <c r="H4" s="8">
+        <v>10</v>
+      </c>
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
       <c r="K4" s="16">
@@ -2871,7 +2875,9 @@
       <c r="L4" s="9">
         <v>10</v>
       </c>
-      <c r="M4" s="9"/>
+      <c r="M4" s="9">
+        <v>10</v>
+      </c>
       <c r="N4" s="9"/>
       <c r="O4" s="9"/>
       <c r="P4" s="13">
@@ -2881,26 +2887,30 @@
       <c r="Q4" s="25">
         <v>10</v>
       </c>
-      <c r="R4" s="25"/>
+      <c r="R4" s="25">
+        <v>9</v>
+      </c>
       <c r="S4" s="25"/>
       <c r="T4" s="25"/>
       <c r="U4" s="26">
         <f>AVERAGE(Q4:T4)</f>
-        <v>10</v>
+        <v>9.5</v>
       </c>
       <c r="V4" s="10">
         <v>10</v>
       </c>
-      <c r="W4" s="10"/>
+      <c r="W4" s="10">
+        <v>9</v>
+      </c>
       <c r="X4" s="10"/>
       <c r="Y4" s="10"/>
       <c r="Z4" s="17">
         <f>AVERAGE(V4:Y4)</f>
-        <v>10</v>
+        <v>9.5</v>
       </c>
       <c r="AA4" s="11">
         <f t="shared" ref="AA4:AA6" si="0">+F4</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AB4" s="29">
         <f>+K4</f>
@@ -2912,15 +2922,15 @@
       </c>
       <c r="AD4" s="29">
         <f>+U4</f>
-        <v>10</v>
+        <v>9.5</v>
       </c>
       <c r="AE4" s="29">
         <f>+Z4</f>
-        <v>10</v>
+        <v>9.5</v>
       </c>
       <c r="AF4" s="18">
         <f t="shared" ref="AF4:AF7" si="1">AVERAGE(AA4:AE4)</f>
-        <v>10</v>
+        <v>9.6</v>
       </c>
     </row>
     <row r="5" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2930,7 +2940,9 @@
       <c r="B5" s="12">
         <v>10</v>
       </c>
-      <c r="C5" s="1"/>
+      <c r="C5" s="1">
+        <v>10</v>
+      </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="15">
@@ -2940,7 +2952,9 @@
       <c r="G5" s="8">
         <v>10</v>
       </c>
-      <c r="H5" s="2"/>
+      <c r="H5" s="2">
+        <v>10</v>
+      </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="16">
@@ -2950,7 +2964,9 @@
       <c r="L5" s="9">
         <v>10</v>
       </c>
-      <c r="M5" s="3"/>
+      <c r="M5" s="3">
+        <v>10</v>
+      </c>
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
       <c r="P5" s="13">
@@ -2960,7 +2976,9 @@
       <c r="Q5" s="25">
         <v>10</v>
       </c>
-      <c r="R5" s="27"/>
+      <c r="R5" s="27">
+        <v>10</v>
+      </c>
       <c r="S5" s="27"/>
       <c r="T5" s="25"/>
       <c r="U5" s="26">
@@ -2970,7 +2988,9 @@
       <c r="V5" s="10">
         <v>10</v>
       </c>
-      <c r="W5" s="4"/>
+      <c r="W5" s="4">
+        <v>10</v>
+      </c>
       <c r="X5" s="4"/>
       <c r="Y5" s="4"/>
       <c r="Z5" s="17">
@@ -3009,7 +3029,9 @@
       <c r="B6" s="12">
         <v>10</v>
       </c>
-      <c r="C6" s="1"/>
+      <c r="C6" s="1">
+        <v>10</v>
+      </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="15">
@@ -3019,7 +3041,9 @@
       <c r="G6" s="8">
         <v>10</v>
       </c>
-      <c r="H6" s="2"/>
+      <c r="H6" s="2">
+        <v>10</v>
+      </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="16">
@@ -3029,7 +3053,9 @@
       <c r="L6" s="9">
         <v>10</v>
       </c>
-      <c r="M6" s="3"/>
+      <c r="M6" s="3">
+        <v>10</v>
+      </c>
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
       <c r="P6" s="13">
@@ -3039,7 +3065,9 @@
       <c r="Q6" s="25">
         <v>10</v>
       </c>
-      <c r="R6" s="27"/>
+      <c r="R6" s="27">
+        <v>10</v>
+      </c>
       <c r="S6" s="27"/>
       <c r="T6" s="25"/>
       <c r="U6" s="26">
@@ -3049,7 +3077,9 @@
       <c r="V6" s="10">
         <v>10</v>
       </c>
-      <c r="W6" s="4"/>
+      <c r="W6" s="4">
+        <v>10</v>
+      </c>
       <c r="X6" s="4"/>
       <c r="Y6" s="4"/>
       <c r="Z6" s="17">
@@ -3112,7 +3142,7 @@
       <c r="Z7" s="23"/>
       <c r="AA7" s="31">
         <f>AVERAGE(AA4:AA6)</f>
-        <v>10</v>
+        <v>9.6666666666666661</v>
       </c>
       <c r="AB7" s="32">
         <f>AVERAGE(AB4:AB6)</f>
@@ -3124,15 +3154,15 @@
       </c>
       <c r="AD7" s="32">
         <f>AVERAGE(AD4:AD6)</f>
-        <v>10</v>
+        <v>9.8333333333333339</v>
       </c>
       <c r="AE7" s="32">
         <f>AVERAGE(AE4:AE6)</f>
-        <v>10</v>
+        <v>9.8333333333333339</v>
       </c>
       <c r="AF7" s="28">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>9.8666666666666671</v>
       </c>
     </row>
   </sheetData>

</xml_diff>